<commit_message>
Update Figma link and user stories file
</commit_message>
<xml_diff>
--- a/user stories.xlsx
+++ b/user stories.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Modele - Projet\Projet-DA-ocrs\Projet - 10 - Learn@Home\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Modele - Projet\Projet-DA-ocrs\Projet-LearnAtHome\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C9D1E9C-054A-4901-8776-6880047CE54F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F32D0401-74ED-4B7B-9A48-C62B0E28E201}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{CA12ACD4-676E-469F-94B7-B7A252523465}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="159">
   <si>
     <t>Je souhaite,</t>
   </si>
@@ -226,12 +226,6 @@
   </si>
   <si>
     <t>le contact est supprimé de ma liste  ainsi que l'historique de notre conversation.</t>
-  </si>
-  <si>
-    <t>je clique sur le bouton "supprimer un contact" et que je ferme la modale de confirmation</t>
-  </si>
-  <si>
-    <t>je clique sur le bouton "supprimer un contact" et que je clique sur "confirmer" dans la modale de confirmation</t>
   </si>
   <si>
     <t>le contact et son historique de conversation est conservé.</t>
@@ -445,33 +439,21 @@
     <t>Ajout d'évènement</t>
   </si>
   <si>
-    <t>Modification d'évènement</t>
-  </si>
-  <si>
     <t>Gestion participant</t>
   </si>
   <si>
     <t>Visualisation de la page</t>
   </si>
   <si>
-    <t>je clique sur "nouvelle tâche" , une modale avec un titre et une description a remplir apparait. Je clique sur "enregistrer"</t>
-  </si>
-  <si>
     <t>archiver un tâche</t>
   </si>
   <si>
     <t>avoir une vision claires des tickets terminés et des tickets restant.</t>
   </si>
   <si>
-    <t>je clique sur l'icone "check vert"</t>
-  </si>
-  <si>
     <t>le ticket est transféré dans la liste des tickets terminés.</t>
   </si>
   <si>
-    <t>je clique sur "nouvelle tâche" , une modale avec un titre et une description a remplir apparait. Je clique sur "X"</t>
-  </si>
-  <si>
     <t>la modale se ferme sans générer de nouveau ticket.</t>
   </si>
   <si>
@@ -557,6 +539,54 @@
   </si>
   <si>
     <t>le mois varie en fonction du chevron cliqué.</t>
+  </si>
+  <si>
+    <t>je clique sur l'icone "X"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">je suis un élève qui supprime une tache </t>
+  </si>
+  <si>
+    <t>la tache a été créé par mon mentor</t>
+  </si>
+  <si>
+    <t>le ticket est indiqué comme terminée sur sa page gestionnaire de tache</t>
+  </si>
+  <si>
+    <t>Scénario  #3</t>
+  </si>
+  <si>
+    <t>je suis sur mon tableau de bord et qu'il ya plus de tickets qu'il y a de place</t>
+  </si>
+  <si>
+    <t>je clique sur le chevron direction droite</t>
+  </si>
+  <si>
+    <t>les tickets suivant s'affichent.</t>
+  </si>
+  <si>
+    <t>je clique sur "nouvelle tâche" , une modale avec une description a remplir apparait. Je clique sur "enregistrer"</t>
+  </si>
+  <si>
+    <t>je clique sur "ajouter une tâche" , une modale avec un titre et une description a remplir apparait. Je clique sur "X"</t>
+  </si>
+  <si>
+    <t>je clique sur "supprimer le contact" et que je clique sur "confirmer" dans la modale de confirmation</t>
+  </si>
+  <si>
+    <t>je clique sur  "supprimer un contact" et que je ferme la modale de confirmation</t>
+  </si>
+  <si>
+    <t>Gestion d'évènement</t>
+  </si>
+  <si>
+    <t>je suis sur la page du calendrier et j'ai sélectionné un évènement</t>
+  </si>
+  <si>
+    <t>je clique sur "supprimer"</t>
+  </si>
+  <si>
+    <t>l'évènement est retiré du calendrier</t>
   </si>
 </sst>
 </file>
@@ -1092,7 +1122,7 @@
   <dimension ref="C1:G196"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1118,11 +1148,11 @@
     </row>
     <row r="2" spans="3:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="17" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="3:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1149,7 +1179,7 @@
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="1" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1161,7 +1191,7 @@
       </c>
       <c r="D7" s="13"/>
       <c r="E7" s="14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="3:7" s="10" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1198,7 +1228,7 @@
       </c>
       <c r="D12" s="13"/>
       <c r="E12" s="14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="3:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1207,7 +1237,7 @@
       </c>
       <c r="D13" s="8"/>
       <c r="E13" s="1" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
     <row r="14" spans="3:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1225,16 +1255,16 @@
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="1" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="18" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C18" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19" spans="3:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -1261,7 +1291,7 @@
       </c>
       <c r="D21" s="8"/>
       <c r="E21" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="3:5" x14ac:dyDescent="0.25">
@@ -1270,7 +1300,7 @@
       </c>
       <c r="D23" s="13"/>
       <c r="E23" s="14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="3:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -1306,7 +1336,7 @@
       </c>
       <c r="D28" s="13"/>
       <c r="E28" s="14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="29" spans="3:5" x14ac:dyDescent="0.25">
@@ -1342,7 +1372,7 @@
       </c>
       <c r="D35" s="3"/>
       <c r="E35" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="36" spans="3:5" x14ac:dyDescent="0.25">
@@ -1378,7 +1408,7 @@
       </c>
       <c r="D40" s="13"/>
       <c r="E40" s="14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="41" spans="3:5" x14ac:dyDescent="0.25">
@@ -1473,7 +1503,7 @@
       </c>
       <c r="D155" s="13"/>
       <c r="E155" s="14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="156" spans="3:5" x14ac:dyDescent="0.25">
@@ -1512,8 +1542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{197520CB-DA96-4D17-B149-5E09824DDBF5}">
   <dimension ref="C1:G196"/>
   <sheetViews>
-    <sheetView topLeftCell="B13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView topLeftCell="B47" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1547,7 +1577,7 @@
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G6" s="11"/>
     </row>
@@ -1575,7 +1605,7 @@
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="3:7" s="10" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1588,7 +1618,7 @@
       </c>
       <c r="D12" s="13"/>
       <c r="E12" s="14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1597,7 +1627,7 @@
       </c>
       <c r="D13" s="8"/>
       <c r="E13" s="1" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
     <row r="14" spans="3:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1620,22 +1650,26 @@
       </c>
       <c r="D17" s="13"/>
       <c r="E17" s="14" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="18" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C18" s="7" t="s">
         <v>2</v>
       </c>
       <c r="D18" s="8"/>
       <c r="E18" s="1" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
     </row>
     <row r="19" spans="3:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="7"/>
+      <c r="C19" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="D19" s="8"/>
-      <c r="E19" s="1"/>
+      <c r="E19" s="1" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="20" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C20" s="7" t="s">
@@ -1643,295 +1677,329 @@
       </c>
       <c r="D20" s="8"/>
       <c r="E20" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="23" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C23" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23" s="3"/>
-      <c r="E23" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="24" spans="3:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C24" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D24" s="6"/>
-      <c r="E24" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="24" spans="3:5" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C25" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D25" s="8"/>
-      <c r="E25" s="1" t="s">
-        <v>33</v>
+      <c r="C25" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D25" s="13"/>
+      <c r="E25" s="14" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="26" spans="3:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C26" s="7" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D26" s="8"/>
       <c r="E26" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="27" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C27" s="7"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C28" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" s="8"/>
+      <c r="E28" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="33" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33" s="3"/>
+      <c r="E33" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="34" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C34" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" s="6"/>
+      <c r="E34" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C35" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D35" s="8"/>
+      <c r="E35" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="C36" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="8"/>
+      <c r="E36" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C29" s="12" t="s">
+    <row r="39" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C39" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D29" s="13"/>
-      <c r="E29" s="14" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="30" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C30" s="7" t="s">
+      <c r="D39" s="13"/>
+      <c r="E39" s="14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="40" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C40" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D30" s="8"/>
-      <c r="E30" s="1" t="s">
+      <c r="D40" s="8"/>
+      <c r="E40" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C31" s="7" t="s">
+    <row r="41" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C41" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D31" s="8"/>
-      <c r="E31" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="32" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C32" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D32" s="8"/>
-      <c r="E32" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="35" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C35" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D35" s="3"/>
-      <c r="E35" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="36" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C36" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D36" s="6"/>
-      <c r="E36" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="37" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C37" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D37" s="8"/>
-      <c r="E37" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="38" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C38" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D38" s="8"/>
-      <c r="E38" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="41" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C41" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="D41" s="13"/>
-      <c r="E41" s="14" t="s">
-        <v>57</v>
+      <c r="D41" s="8"/>
+      <c r="E41" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="42" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C42" s="7" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D42" s="8"/>
       <c r="E42" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="44" spans="3:5" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C45" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D45" s="3"/>
+      <c r="E45" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="46" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C46" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D46" s="6"/>
+      <c r="E46" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="47" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C47" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D47" s="8"/>
+      <c r="E47" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="48" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C48" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D48" s="8"/>
+      <c r="E48" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="51" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C51" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D51" s="13"/>
+      <c r="E51" s="14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="52" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C52" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D52" s="8"/>
+      <c r="E52" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="43" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C43" s="7" t="s">
+    <row r="53" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C53" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D43" s="8"/>
-      <c r="E43" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="44" spans="3:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C44" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D44" s="8"/>
-      <c r="E44" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="47" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C47" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D47" s="3"/>
-      <c r="E47" s="4" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="48" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C48" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D48" s="6"/>
-      <c r="E48" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="49" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C49" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D49" s="8"/>
-      <c r="E49" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="50" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C50" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D50" s="8"/>
-      <c r="E50" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="53" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C53" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="D53" s="13"/>
-      <c r="E53" s="14" t="s">
-        <v>57</v>
+      <c r="D53" s="8"/>
+      <c r="E53" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="54" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C54" s="7" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D54" s="8"/>
       <c r="E54" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="57" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C57" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D57" s="3"/>
+      <c r="E57" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="58" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C58" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D58" s="6"/>
+      <c r="E58" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="59" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C59" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D59" s="8"/>
+      <c r="E59" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="60" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C60" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D60" s="8"/>
+      <c r="E60" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="63" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C63" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D63" s="13"/>
+      <c r="E63" s="14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="64" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C64" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D64" s="8"/>
+      <c r="E64" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="55" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C55" s="7" t="s">
+    <row r="65" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C65" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D55" s="8"/>
-      <c r="E55" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="56" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C56" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D56" s="8"/>
-      <c r="E56" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="59" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C59" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D59" s="3"/>
-      <c r="E59" s="4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="60" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C60" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D60" s="6"/>
-      <c r="E60" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="61" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C61" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D61" s="8"/>
-      <c r="E61" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="62" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C62" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D62" s="8"/>
-      <c r="E62" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="65" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C65" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="D65" s="13"/>
-      <c r="E65" s="14" t="s">
-        <v>57</v>
+      <c r="D65" s="8"/>
+      <c r="E65" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="66" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C66" s="7" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D66" s="8"/>
       <c r="E66" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="69" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C69" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D69" s="3"/>
+      <c r="E69" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="70" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C70" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D70" s="6"/>
+      <c r="E70" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="71" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C71" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D71" s="8"/>
+      <c r="E71" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="72" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C72" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D72" s="8"/>
+      <c r="E72" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="75" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C75" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D75" s="13"/>
+      <c r="E75" s="14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="76" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C76" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D76" s="8"/>
+      <c r="E76" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="67" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C67" s="7" t="s">
+    <row r="77" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C77" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D67" s="8"/>
-      <c r="E67" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="68" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C68" s="7" t="s">
+      <c r="D77" s="8"/>
+      <c r="E77" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="78" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C78" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D68" s="8"/>
-      <c r="E68" s="1" t="s">
-        <v>77</v>
+      <c r="D78" s="8"/>
+      <c r="E78" s="1" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="159" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -1998,7 +2066,7 @@
       </c>
       <c r="D173" s="13"/>
       <c r="E173" s="14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="174" spans="3:5" x14ac:dyDescent="0.25">
@@ -2037,8 +2105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAC8C352-D861-4727-BE2B-A83173A95B7E}">
   <dimension ref="C1:G196"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView topLeftCell="B13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2071,7 +2139,7 @@
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2111,7 +2179,7 @@
       </c>
       <c r="D10" s="13"/>
       <c r="E10" s="14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2129,7 +2197,7 @@
       </c>
       <c r="D12" s="8"/>
       <c r="E12" s="1" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="13" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2138,7 +2206,7 @@
       </c>
       <c r="D13" s="8"/>
       <c r="E13" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="14" spans="3:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2148,7 +2216,7 @@
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.25">
@@ -2184,7 +2252,7 @@
       </c>
       <c r="D21" s="13"/>
       <c r="E21" s="14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="3:5" x14ac:dyDescent="0.25">
@@ -2202,7 +2270,7 @@
       </c>
       <c r="D23" s="8"/>
       <c r="E23" s="1" t="s">
-        <v>55</v>
+        <v>153</v>
       </c>
     </row>
     <row r="24" spans="3:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -2220,7 +2288,7 @@
       </c>
       <c r="D26" s="13"/>
       <c r="E26" s="14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" spans="3:5" x14ac:dyDescent="0.25">
@@ -2232,13 +2300,13 @@
         <v>49</v>
       </c>
     </row>
-    <row r="28" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C28" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D28" s="8"/>
       <c r="E28" s="1" t="s">
-        <v>54</v>
+        <v>154</v>
       </c>
     </row>
     <row r="29" spans="3:5" x14ac:dyDescent="0.25">
@@ -2247,7 +2315,7 @@
       </c>
       <c r="D29" s="8"/>
       <c r="E29" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="32" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -2256,7 +2324,7 @@
       </c>
       <c r="D32" s="3"/>
       <c r="E32" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="33" spans="3:5" x14ac:dyDescent="0.25">
@@ -2274,7 +2342,7 @@
       </c>
       <c r="D34" s="8"/>
       <c r="E34" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="35" spans="3:5" x14ac:dyDescent="0.25">
@@ -2283,7 +2351,7 @@
       </c>
       <c r="D35" s="8"/>
       <c r="E35" s="1" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="37" spans="3:5" x14ac:dyDescent="0.25">
@@ -2292,7 +2360,7 @@
       </c>
       <c r="D37" s="13"/>
       <c r="E37" s="14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="38" spans="3:5" x14ac:dyDescent="0.25">
@@ -2319,7 +2387,7 @@
       </c>
       <c r="D40" s="8"/>
       <c r="E40" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="44" spans="3:5" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2387,7 +2455,7 @@
       </c>
       <c r="D161" s="13"/>
       <c r="E161" s="14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="162" spans="3:5" x14ac:dyDescent="0.25">
@@ -2426,8 +2494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB3A201B-F358-4D06-B8B3-C99A08171D40}">
   <dimension ref="C1:G196"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I59" sqref="I59"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2461,7 +2529,7 @@
     </row>
     <row r="10" spans="3:7" s="10" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D10" s="18"/>
       <c r="E10" s="18"/>
@@ -2472,7 +2540,7 @@
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2481,7 +2549,7 @@
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2490,7 +2558,7 @@
       </c>
       <c r="D13" s="8"/>
       <c r="E13" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="3:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -2499,7 +2567,7 @@
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.25">
@@ -2508,7 +2576,7 @@
       </c>
       <c r="D17" s="13"/>
       <c r="E17" s="14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="3:5" x14ac:dyDescent="0.25">
@@ -2517,7 +2585,7 @@
       </c>
       <c r="D18" s="8"/>
       <c r="E18" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="3:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -2526,7 +2594,7 @@
       </c>
       <c r="D19" s="8"/>
       <c r="E19" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="3:5" ht="30" x14ac:dyDescent="0.25">
@@ -2535,7 +2603,7 @@
       </c>
       <c r="D20" s="8"/>
       <c r="E20" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -2544,7 +2612,7 @@
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="4" t="s">
-        <v>111</v>
+        <v>155</v>
       </c>
     </row>
     <row r="24" spans="3:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -2553,7 +2621,7 @@
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="3:5" x14ac:dyDescent="0.25">
@@ -2562,7 +2630,7 @@
       </c>
       <c r="D25" s="8"/>
       <c r="E25" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="26" spans="3:5" x14ac:dyDescent="0.25">
@@ -2571,7 +2639,7 @@
       </c>
       <c r="D26" s="8"/>
       <c r="E26" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" spans="3:5" x14ac:dyDescent="0.25">
@@ -2580,7 +2648,7 @@
       </c>
       <c r="D29" s="13"/>
       <c r="E29" s="14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="3:5" x14ac:dyDescent="0.25">
@@ -2589,7 +2657,7 @@
       </c>
       <c r="D30" s="8"/>
       <c r="E30" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31" spans="3:5" x14ac:dyDescent="0.25">
@@ -2598,7 +2666,7 @@
       </c>
       <c r="D31" s="8"/>
       <c r="E31" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="32" spans="3:5" x14ac:dyDescent="0.25">
@@ -2607,187 +2675,224 @@
       </c>
       <c r="D32" s="8"/>
       <c r="E32" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="35" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C35" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D35" s="3"/>
-      <c r="E35" s="4" t="s">
-        <v>112</v>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="34" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C34" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D34" s="13"/>
+      <c r="E34" s="14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C35" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D35" s="8"/>
+      <c r="E35" s="1" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="36" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C36" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D36" s="6"/>
+      <c r="C36" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D36" s="8"/>
       <c r="E36" s="1" t="s">
-        <v>88</v>
+        <v>157</v>
       </c>
     </row>
     <row r="37" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C37" s="7" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D37" s="8"/>
       <c r="E37" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="38" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C38" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D38" s="8"/>
-      <c r="E38" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="41" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C41" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="D41" s="13"/>
-      <c r="E41" s="14" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="42" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C42" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D42" s="8"/>
-      <c r="E42" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="43" spans="3:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="C43" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D43" s="8"/>
-      <c r="E43" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="44" spans="3:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C44" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D44" s="8"/>
-      <c r="E44" s="1" t="s">
-        <v>84</v>
+        <v>158</v>
+      </c>
+    </row>
+    <row r="44" spans="3:5" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C45" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D45" s="3"/>
+      <c r="E45" s="4" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="46" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C46" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="D46" s="13"/>
-      <c r="E46" s="14" t="s">
-        <v>58</v>
+      <c r="C46" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D46" s="6"/>
+      <c r="E46" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="47" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C47" s="7" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D47" s="8"/>
       <c r="E47" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="48" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C48" s="7" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D48" s="8"/>
       <c r="E48" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="49" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C49" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D49" s="8"/>
-      <c r="E49" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="52" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C52" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D52" s="3"/>
-      <c r="E52" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="53" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C53" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D53" s="6"/>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="51" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C51" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D51" s="13"/>
+      <c r="E51" s="14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="52" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C52" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D52" s="8"/>
+      <c r="E52" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="53" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="C53" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D53" s="8"/>
       <c r="E53" s="1" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
     </row>
     <row r="54" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C54" s="7" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D54" s="8"/>
       <c r="E54" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="55" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C55" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D55" s="8"/>
-      <c r="E55" s="1" t="s">
-        <v>146</v>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="56" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C56" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D56" s="13"/>
+      <c r="E56" s="14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="57" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C57" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D57" s="8"/>
+      <c r="E57" s="1" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="58" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C58" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="D58" s="13"/>
-      <c r="E58" s="14" t="s">
-        <v>57</v>
+      <c r="C58" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D58" s="8"/>
+      <c r="E58" s="1" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="59" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C59" s="7" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D59" s="8"/>
       <c r="E59" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="60" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C60" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="62" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C62" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D62" s="3"/>
+      <c r="E62" s="4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="63" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C63" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D63" s="6"/>
+      <c r="E63" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="64" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C64" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D64" s="8"/>
+      <c r="E64" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="65" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C65" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D65" s="8"/>
+      <c r="E65" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="68" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C68" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D68" s="13"/>
+      <c r="E68" s="14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="69" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C69" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D69" s="8"/>
+      <c r="E69" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="70" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C70" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D60" s="8"/>
-      <c r="E60" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="61" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C61" s="7" t="s">
+      <c r="D70" s="8"/>
+      <c r="E70" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="71" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C71" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D61" s="8"/>
-      <c r="E61" s="1" t="s">
-        <v>148</v>
+      <c r="D71" s="8"/>
+      <c r="E71" s="1" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="150" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -2854,7 +2959,7 @@
       </c>
       <c r="D164" s="13"/>
       <c r="E164" s="14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="165" spans="3:5" x14ac:dyDescent="0.25">
@@ -2893,8 +2998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25EFA7AE-1195-4A8D-AD82-3E3C2504A216}">
   <dimension ref="C1:G196"/>
   <sheetViews>
-    <sheetView topLeftCell="B13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I54" sqref="I53:I54"/>
+    <sheetView topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E64" sqref="E64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2916,18 +3021,18 @@
     <row r="3" spans="3:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="3:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="18" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D4" s="18"/>
       <c r="E4" s="18"/>
     </row>
     <row r="5" spans="3:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2936,7 +3041,7 @@
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G6" s="11"/>
     </row>
@@ -2946,7 +3051,7 @@
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="1" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="3:7" s="10" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -2955,7 +3060,7 @@
       </c>
       <c r="D8" s="8"/>
       <c r="E8" s="1" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="3:7" s="10" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2970,7 +3075,7 @@
       </c>
       <c r="D11" s="13"/>
       <c r="E11" s="14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2979,7 +3084,7 @@
       </c>
       <c r="D12" s="8"/>
       <c r="E12" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2993,7 +3098,7 @@
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="1" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16" spans="3:7" x14ac:dyDescent="0.25">
@@ -3002,7 +3107,7 @@
       </c>
       <c r="D16" s="13"/>
       <c r="E16" s="14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.25">
@@ -3011,7 +3116,7 @@
       </c>
       <c r="D17" s="8"/>
       <c r="E17" s="1" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
     </row>
     <row r="18" spans="3:5" x14ac:dyDescent="0.25">
@@ -3025,16 +3130,16 @@
       </c>
       <c r="D19" s="8"/>
       <c r="E19" s="1" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="22" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C22" s="16" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="3:5" x14ac:dyDescent="0.25">
@@ -3043,7 +3148,7 @@
       </c>
       <c r="D23" s="6"/>
       <c r="E23" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="3:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -3052,7 +3157,7 @@
       </c>
       <c r="D24" s="8"/>
       <c r="E24" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25" spans="3:5" x14ac:dyDescent="0.25">
@@ -3061,7 +3166,7 @@
       </c>
       <c r="D25" s="8"/>
       <c r="E25" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="28" spans="3:5" x14ac:dyDescent="0.25">
@@ -3070,7 +3175,7 @@
       </c>
       <c r="D28" s="13"/>
       <c r="E28" s="14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="3:5" x14ac:dyDescent="0.25">
@@ -3079,7 +3184,7 @@
       </c>
       <c r="D29" s="8"/>
       <c r="E29" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="30" spans="3:5" ht="30" x14ac:dyDescent="0.25">
@@ -3088,7 +3193,7 @@
       </c>
       <c r="D30" s="8"/>
       <c r="E30" s="1" t="s">
-        <v>114</v>
+        <v>151</v>
       </c>
     </row>
     <row r="31" spans="3:5" x14ac:dyDescent="0.25">
@@ -3097,7 +3202,7 @@
       </c>
       <c r="D31" s="8"/>
       <c r="E31" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="33" spans="3:5" x14ac:dyDescent="0.25">
@@ -3106,7 +3211,7 @@
       </c>
       <c r="D33" s="13"/>
       <c r="E33" s="14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="34" spans="3:5" x14ac:dyDescent="0.25">
@@ -3115,7 +3220,7 @@
       </c>
       <c r="D34" s="8"/>
       <c r="E34" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="35" spans="3:5" ht="30" x14ac:dyDescent="0.25">
@@ -3124,7 +3229,7 @@
       </c>
       <c r="D35" s="8"/>
       <c r="E35" s="1" t="s">
-        <v>119</v>
+        <v>152</v>
       </c>
     </row>
     <row r="36" spans="3:5" x14ac:dyDescent="0.25">
@@ -3133,16 +3238,16 @@
       </c>
       <c r="D36" s="8"/>
       <c r="E36" s="1" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="39" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C39" s="15" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D39" s="3"/>
       <c r="E39" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="40" spans="3:5" x14ac:dyDescent="0.25">
@@ -3151,7 +3256,7 @@
       </c>
       <c r="D40" s="6"/>
       <c r="E40" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="41" spans="3:5" x14ac:dyDescent="0.25">
@@ -3160,7 +3265,7 @@
       </c>
       <c r="D41" s="8"/>
       <c r="E41" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="42" spans="3:5" x14ac:dyDescent="0.25">
@@ -3169,7 +3274,7 @@
       </c>
       <c r="D42" s="8"/>
       <c r="E42" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="44" spans="3:5" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3179,7 +3284,7 @@
       </c>
       <c r="D45" s="13"/>
       <c r="E45" s="14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="46" spans="3:5" x14ac:dyDescent="0.25">
@@ -3188,7 +3293,7 @@
       </c>
       <c r="D46" s="8"/>
       <c r="E46" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="47" spans="3:5" x14ac:dyDescent="0.25">
@@ -3197,7 +3302,7 @@
       </c>
       <c r="D47" s="8"/>
       <c r="E47" s="1" t="s">
-        <v>117</v>
+        <v>143</v>
       </c>
     </row>
     <row r="48" spans="3:5" x14ac:dyDescent="0.25">
@@ -3206,79 +3311,115 @@
       </c>
       <c r="D48" s="8"/>
       <c r="E48" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="51" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C51" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="D51" s="3"/>
-      <c r="E51" s="4" t="s">
-        <v>121</v>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="50" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C50" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D50" s="13"/>
+      <c r="E50" s="14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="51" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C51" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D51" s="8"/>
+      <c r="E51" s="1" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="52" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C52" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D52" s="6"/>
+      <c r="C52" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D52" s="8"/>
       <c r="E52" s="1" t="s">
-        <v>122</v>
+        <v>145</v>
       </c>
     </row>
     <row r="53" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C53" s="7" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D53" s="8"/>
       <c r="E53" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="54" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C54" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D54" s="8"/>
-      <c r="E54" s="1" t="s">
-        <v>137</v>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="56" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C56" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="D56" s="3"/>
+      <c r="E56" s="4" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="57" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C57" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="D57" s="13"/>
-      <c r="E57" s="14" t="s">
-        <v>57</v>
+      <c r="C57" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D57" s="6"/>
+      <c r="E57" s="1" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="58" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C58" s="7" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D58" s="8"/>
       <c r="E58" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="59" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="59" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C59" s="7" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D59" s="8"/>
       <c r="E59" s="1" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="60" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C60" s="7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="62" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C62" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D62" s="13"/>
+      <c r="E62" s="14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="63" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C63" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D63" s="8"/>
+      <c r="E63" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="64" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="C64" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D64" s="8"/>
+      <c r="E64" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="65" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C65" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D60" s="8"/>
-      <c r="E60" s="1" t="s">
-        <v>139</v>
+      <c r="D65" s="8"/>
+      <c r="E65" s="1" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="158" spans="3:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -3345,7 +3486,7 @@
       </c>
       <c r="D172" s="13"/>
       <c r="E172" s="14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="173" spans="3:5" x14ac:dyDescent="0.25">

</xml_diff>